<commit_message>
profile page done 24-5-2024
</commit_message>
<xml_diff>
--- a/myWorkRecord.xlsx
+++ b/myWorkRecord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\company_workStatus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D62F13B-F439-4963-AD7D-984DCE2D21F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C960C1-942D-409A-A0FB-E474F4B438CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B17A294C-326E-4CE6-969D-DF31A9FF5360}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
   <si>
     <t>sr no</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>creating a profile page ui</t>
   </si>
 </sst>
 </file>
@@ -463,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD9B361-BF5A-439E-8D42-125E33476358}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,6 +770,12 @@
       <c r="B19" s="1">
         <v>45436</v>
       </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">

</xml_diff>

<commit_message>
28-5-2024 create category list done
</commit_message>
<xml_diff>
--- a/myWorkRecord.xlsx
+++ b/myWorkRecord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\company_workStatus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D429FE2D-BD85-4927-92ED-E2C6992266F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B7E636-7D1A-44FD-AA65-95872C377830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="1860" windowWidth="15375" windowHeight="7875" xr2:uid="{B17A294C-326E-4CE6-969D-DF31A9FF5360}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="28">
   <si>
     <t>sr no</t>
   </si>
@@ -105,7 +105,10 @@
     <t>creating a profile page ui</t>
   </si>
   <si>
-    <t>changes butto text color</t>
+    <t>make category component and make routing and make table with search bar and add button</t>
+  </si>
+  <si>
+    <t>changes button text color</t>
   </si>
 </sst>
 </file>
@@ -467,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD9B361-BF5A-439E-8D42-125E33476358}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="C17" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,7 +791,7 @@
         <v>45439</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D20" t="s">
         <v>24</v>
@@ -803,6 +806,23 @@
       </c>
       <c r="B21" s="1">
         <v>45440</v>
+      </c>
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>45441</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
4-06-2024 work done in half day
</commit_message>
<xml_diff>
--- a/myWorkRecord.xlsx
+++ b/myWorkRecord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\company_workStatus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4FC242-70DB-425D-B0C2-6B6FF8C7FA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D59E2A3-A918-4B1B-B44E-337B8143B9F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B17A294C-326E-4CE6-969D-DF31A9FF5360}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="34">
   <si>
     <t>sr no</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>make navlink dashboad and it conditionly render then add content as card and make it responsive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">make profile menu list profile and logout and add icon on dashboard and fixed ipad mini sized </t>
+  </si>
+  <si>
+    <t>half day</t>
   </si>
 </sst>
 </file>
@@ -485,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD9B361-BF5A-439E-8D42-125E33476358}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="D18" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -910,6 +916,15 @@
       <c r="B30" s="1">
         <v>45447</v>
       </c>
+      <c r="C30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">

</xml_diff>

<commit_message>
5 & 6 jun work done
</commit_message>
<xml_diff>
--- a/myWorkRecord.xlsx
+++ b/myWorkRecord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\company_workStatus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D59E2A3-A918-4B1B-B44E-337B8143B9F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CDFEA8-FF65-48F7-8D8D-590B53675D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B17A294C-326E-4CE6-969D-DF31A9FF5360}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="36">
   <si>
     <t>sr no</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>half day</t>
+  </si>
+  <si>
+    <t>fixed button add &amp; edit component in dashboard card icon title and add menu design and conditionaly render the proper value</t>
+  </si>
+  <si>
+    <t>make another 4 card different design and first card in one row and other are 1 row 2 card</t>
   </si>
 </sst>
 </file>
@@ -491,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD9B361-BF5A-439E-8D42-125E33476358}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D18" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,6 +939,15 @@
       <c r="B31" s="1">
         <v>45448</v>
       </c>
+      <c r="C31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
@@ -940,6 +955,15 @@
       </c>
       <c r="B32" s="1">
         <v>45449</v>
+      </c>
+      <c r="C32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>